<commit_message>
added steps in LinkedinSearchResultsTest
</commit_message>
<xml_diff>
--- a/src/test/java/com/qa/linkedin/data/TestData.xlsx
+++ b/src/test/java/com/qa/linkedin/data/TestData.xlsx
@@ -16,18 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>SearchText</t>
   </si>
   <si>
     <t>Ramesh</t>
-  </si>
-  <si>
-    <t>Robin</t>
-  </si>
-  <si>
-    <t>Reehan</t>
   </si>
   <si>
     <t>Rahul</t>
@@ -369,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,16 +389,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>